<commit_message>
changed the merge function
</commit_message>
<xml_diff>
--- a/errors.xlsx
+++ b/errors.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8550" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8550" uniqueCount="167">
   <si>
     <t>ToxBatch</t>
   </si>
@@ -508,6 +508,21 @@
   <si>
     <t>B18-8391</t>
   </si>
+  <si>
+    <t>Neanthes arenaceodentata</t>
+  </si>
+  <si>
+    <t>Los Angeles County Sanitation Districts</t>
+  </si>
+  <si>
+    <t>jordon</t>
+  </si>
+  <si>
+    <t>B18-8353</t>
+  </si>
+  <si>
+    <t>B18-8325</t>
+  </si>
 </sst>
 </file>
 
@@ -1074,8 +1089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.5" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,7 +1174,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>35</v>
+        <v>165</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>16</v>
@@ -1171,10 +1186,10 @@
         <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>14</v>
+        <v>164</v>
       </c>
       <c r="G2" s="3">
         <v>-88</v>
@@ -1215,7 +1230,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>35</v>
+        <v>166</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>16</v>
@@ -1227,10 +1242,10 @@
         <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G3" s="3">
         <v>-88</v>
@@ -1283,10 +1298,10 @@
         <v>17</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G4" s="3">
         <v>-88</v>
@@ -1339,10 +1354,10 @@
         <v>17</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G5" s="3">
         <v>-88</v>
@@ -1395,10 +1410,10 @@
         <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G6" s="3">
         <v>-88</v>
@@ -1451,10 +1466,10 @@
         <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G7" s="3">
         <v>-88</v>
@@ -1507,10 +1522,10 @@
         <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G8" s="3">
         <v>-88</v>
@@ -1563,10 +1578,10 @@
         <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G9" s="3">
         <v>-88</v>
@@ -1619,10 +1634,10 @@
         <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G10" s="3">
         <v>-88</v>
@@ -1675,10 +1690,10 @@
         <v>17</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G11" s="3">
         <v>-88</v>
@@ -1731,10 +1746,10 @@
         <v>17</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G12" s="3">
         <v>-88</v>
@@ -1787,10 +1802,10 @@
         <v>17</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G13" s="3">
         <v>-88</v>
@@ -1843,10 +1858,10 @@
         <v>17</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G14" s="3">
         <v>-88</v>
@@ -1899,10 +1914,10 @@
         <v>17</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G15" s="3">
         <v>-88</v>
@@ -1955,10 +1970,10 @@
         <v>17</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G16" s="3">
         <v>-88</v>
@@ -2011,10 +2026,10 @@
         <v>17</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G17" s="3">
         <v>-88</v>
@@ -2067,10 +2082,10 @@
         <v>17</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G18" s="3">
         <v>-88</v>
@@ -2123,10 +2138,10 @@
         <v>17</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G19" s="3">
         <v>-88</v>
@@ -2179,10 +2194,10 @@
         <v>17</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G20" s="3">
         <v>-88</v>
@@ -2235,10 +2250,10 @@
         <v>17</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G21" s="3">
         <v>-88</v>
@@ -2291,10 +2306,10 @@
         <v>17</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G22" s="3">
         <v>-88</v>
@@ -2347,10 +2362,10 @@
         <v>17</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G23" s="3">
         <v>-88</v>
@@ -2403,10 +2418,10 @@
         <v>17</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G24" s="3">
         <v>-88</v>
@@ -2459,10 +2474,10 @@
         <v>17</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G25" s="3">
         <v>-88</v>
@@ -2515,10 +2530,10 @@
         <v>17</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G26" s="3">
         <v>-88</v>
@@ -2571,10 +2586,10 @@
         <v>17</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G27" s="3">
         <v>-88</v>
@@ -2627,10 +2642,10 @@
         <v>17</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G28" s="3">
         <v>-88</v>
@@ -2683,10 +2698,10 @@
         <v>17</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G29" s="3">
         <v>-88</v>
@@ -2739,10 +2754,10 @@
         <v>17</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G30" s="3">
         <v>-88</v>
@@ -2795,10 +2810,10 @@
         <v>17</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G31" s="3">
         <v>-88</v>
@@ -2851,10 +2866,10 @@
         <v>17</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G32" s="3">
         <v>-88</v>
@@ -2907,10 +2922,10 @@
         <v>17</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G33" s="3">
         <v>-88</v>
@@ -2963,10 +2978,10 @@
         <v>17</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G34" s="3">
         <v>-88</v>
@@ -3019,10 +3034,10 @@
         <v>17</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G35" s="3">
         <v>-88</v>
@@ -3075,10 +3090,10 @@
         <v>17</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G36" s="3">
         <v>-88</v>
@@ -3131,10 +3146,10 @@
         <v>17</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G37" s="3">
         <v>-88</v>
@@ -3187,10 +3202,10 @@
         <v>17</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G38" s="3">
         <v>-88</v>
@@ -3243,10 +3258,10 @@
         <v>17</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G39" s="3">
         <v>-88</v>
@@ -3299,10 +3314,10 @@
         <v>17</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G40" s="3">
         <v>-88</v>
@@ -3355,10 +3370,10 @@
         <v>17</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G41" s="3">
         <v>-88</v>
@@ -3411,10 +3426,10 @@
         <v>17</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G42" s="3">
         <v>-88</v>
@@ -3467,10 +3482,10 @@
         <v>17</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G43" s="3">
         <v>-88</v>
@@ -3523,10 +3538,10 @@
         <v>17</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G44" s="3">
         <v>-88</v>
@@ -3579,10 +3594,10 @@
         <v>17</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G45" s="3">
         <v>-88</v>
@@ -3635,10 +3650,10 @@
         <v>17</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G46" s="3">
         <v>-88</v>
@@ -3691,10 +3706,10 @@
         <v>17</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G47" s="3">
         <v>-88</v>
@@ -3747,10 +3762,10 @@
         <v>17</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G48" s="3">
         <v>-88</v>
@@ -3803,10 +3818,10 @@
         <v>17</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G49" s="3">
         <v>-88</v>
@@ -3859,10 +3874,10 @@
         <v>17</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G50" s="3">
         <v>-88</v>
@@ -3915,10 +3930,10 @@
         <v>17</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G51" s="3">
         <v>-88</v>
@@ -3971,10 +3986,10 @@
         <v>17</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G52" s="3">
         <v>-88</v>
@@ -4027,10 +4042,10 @@
         <v>17</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G53" s="3">
         <v>-88</v>
@@ -4083,10 +4098,10 @@
         <v>17</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G54" s="3">
         <v>-88</v>
@@ -4139,10 +4154,10 @@
         <v>17</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G55" s="3">
         <v>-88</v>
@@ -4195,10 +4210,10 @@
         <v>17</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G56" s="3">
         <v>-88</v>
@@ -4251,10 +4266,10 @@
         <v>17</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G57" s="3">
         <v>-88</v>
@@ -4307,10 +4322,10 @@
         <v>17</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G58" s="3">
         <v>-88</v>
@@ -4363,10 +4378,10 @@
         <v>17</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G59" s="3">
         <v>-88</v>
@@ -4419,10 +4434,10 @@
         <v>17</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G60" s="3">
         <v>-88</v>
@@ -4475,10 +4490,10 @@
         <v>17</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G61" s="3">
         <v>-88</v>
@@ -4531,10 +4546,10 @@
         <v>21</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G62" s="3">
         <v>-88</v>
@@ -4587,10 +4602,10 @@
         <v>21</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G63" s="3">
         <v>-88</v>
@@ -4643,10 +4658,10 @@
         <v>21</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G64" s="3">
         <v>-88</v>
@@ -4699,10 +4714,10 @@
         <v>21</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G65" s="3">
         <v>-88</v>
@@ -4755,10 +4770,10 @@
         <v>21</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G66" s="3">
         <v>-88</v>
@@ -4811,10 +4826,10 @@
         <v>21</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G67" s="3">
         <v>-88</v>
@@ -4867,10 +4882,10 @@
         <v>21</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G68" s="3">
         <v>-88</v>
@@ -4923,10 +4938,10 @@
         <v>21</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G69" s="3">
         <v>-88</v>
@@ -4979,10 +4994,10 @@
         <v>21</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G70" s="3">
         <v>-88</v>
@@ -5035,10 +5050,10 @@
         <v>21</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G71" s="3">
         <v>-88</v>
@@ -5091,10 +5106,10 @@
         <v>21</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G72" s="3">
         <v>-88</v>
@@ -5147,10 +5162,10 @@
         <v>21</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G73" s="3">
         <v>-88</v>
@@ -5203,10 +5218,10 @@
         <v>21</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G74" s="3">
         <v>-88</v>
@@ -5259,10 +5274,10 @@
         <v>21</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G75" s="3">
         <v>-88</v>
@@ -5315,10 +5330,10 @@
         <v>21</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G76" s="3">
         <v>-88</v>
@@ -5371,10 +5386,10 @@
         <v>21</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G77" s="3">
         <v>-88</v>
@@ -5427,10 +5442,10 @@
         <v>21</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G78" s="3">
         <v>-88</v>
@@ -5483,10 +5498,10 @@
         <v>21</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G79" s="3">
         <v>-88</v>
@@ -5539,10 +5554,10 @@
         <v>21</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G80" s="3">
         <v>-88</v>
@@ -5595,10 +5610,10 @@
         <v>21</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G81" s="3">
         <v>-88</v>
@@ -5651,10 +5666,10 @@
         <v>21</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G82" s="3">
         <v>-88</v>
@@ -5707,10 +5722,10 @@
         <v>21</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G83" s="3">
         <v>-88</v>
@@ -5763,10 +5778,10 @@
         <v>21</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G84" s="3">
         <v>-88</v>
@@ -5819,10 +5834,10 @@
         <v>21</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G85" s="3">
         <v>-88</v>
@@ -5875,10 +5890,10 @@
         <v>21</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G86" s="3">
         <v>-88</v>
@@ -5931,10 +5946,10 @@
         <v>21</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G87" s="3">
         <v>-88</v>
@@ -5987,10 +6002,10 @@
         <v>21</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G88" s="3">
         <v>-88</v>
@@ -6043,10 +6058,10 @@
         <v>21</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G89" s="3">
         <v>-88</v>
@@ -6099,10 +6114,10 @@
         <v>21</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G90" s="3">
         <v>-88</v>
@@ -6155,10 +6170,10 @@
         <v>21</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G91" s="3">
         <v>-88</v>
@@ -6211,10 +6226,10 @@
         <v>21</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G92" s="3">
         <v>-88</v>
@@ -6267,10 +6282,10 @@
         <v>21</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G93" s="3">
         <v>-88</v>
@@ -6323,10 +6338,10 @@
         <v>21</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G94" s="3">
         <v>-88</v>
@@ -6379,10 +6394,10 @@
         <v>21</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G95" s="3">
         <v>-88</v>
@@ -6435,10 +6450,10 @@
         <v>21</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G96" s="3">
         <v>-88</v>
@@ -6491,10 +6506,10 @@
         <v>21</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G97" s="3">
         <v>-88</v>
@@ -6547,10 +6562,10 @@
         <v>21</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G98" s="3">
         <v>-88</v>
@@ -6603,10 +6618,10 @@
         <v>21</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G99" s="3">
         <v>-88</v>
@@ -6659,10 +6674,10 @@
         <v>21</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G100" s="3">
         <v>-88</v>
@@ -6715,10 +6730,10 @@
         <v>21</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G101" s="3">
         <v>-88</v>
@@ -6771,10 +6786,10 @@
         <v>21</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G102" s="3">
         <v>-88</v>
@@ -6827,10 +6842,10 @@
         <v>21</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G103" s="3">
         <v>-88</v>
@@ -6883,10 +6898,10 @@
         <v>21</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F104" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G104" s="3">
         <v>-88</v>
@@ -6939,10 +6954,10 @@
         <v>21</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G105" s="3">
         <v>-88</v>
@@ -6995,10 +7010,10 @@
         <v>21</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F106" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G106" s="3">
         <v>-88</v>
@@ -7051,10 +7066,10 @@
         <v>21</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F107" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G107" s="3">
         <v>-88</v>
@@ -7107,10 +7122,10 @@
         <v>21</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F108" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G108" s="3">
         <v>-88</v>
@@ -7163,10 +7178,10 @@
         <v>21</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G109" s="3">
         <v>-88</v>
@@ -7219,10 +7234,10 @@
         <v>21</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F110" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G110" s="3">
         <v>-88</v>
@@ -7275,10 +7290,10 @@
         <v>21</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F111" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G111" s="3">
         <v>-88</v>
@@ -7331,10 +7346,10 @@
         <v>21</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F112" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G112" s="3">
         <v>-88</v>
@@ -7387,10 +7402,10 @@
         <v>21</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G113" s="3">
         <v>-88</v>
@@ -7443,10 +7458,10 @@
         <v>21</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G114" s="3">
         <v>-88</v>
@@ -7499,10 +7514,10 @@
         <v>21</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G115" s="3">
         <v>-88</v>
@@ -7555,10 +7570,10 @@
         <v>21</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G116" s="3">
         <v>-88</v>
@@ -7611,10 +7626,10 @@
         <v>21</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G117" s="3">
         <v>-88</v>
@@ -7667,10 +7682,10 @@
         <v>21</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F118" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G118" s="3">
         <v>-88</v>
@@ -7723,10 +7738,10 @@
         <v>21</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F119" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G119" s="3">
         <v>-88</v>
@@ -7779,10 +7794,10 @@
         <v>21</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F120" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G120" s="3">
         <v>-88</v>
@@ -7835,10 +7850,10 @@
         <v>21</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F121" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G121" s="3">
         <v>-88</v>
@@ -7891,10 +7906,10 @@
         <v>21</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F122" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G122" s="3">
         <v>-88</v>
@@ -7947,10 +7962,10 @@
         <v>21</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F123" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G123" s="3">
         <v>-88</v>
@@ -8003,10 +8018,10 @@
         <v>21</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F124" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G124" s="3">
         <v>-88</v>
@@ -8059,10 +8074,10 @@
         <v>21</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F125" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G125" s="3">
         <v>-88</v>
@@ -8115,10 +8130,10 @@
         <v>21</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F126" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G126" s="3">
         <v>-88</v>
@@ -8171,10 +8186,10 @@
         <v>21</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F127" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G127" s="3">
         <v>-88</v>
@@ -8227,10 +8242,10 @@
         <v>21</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F128" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G128" s="3">
         <v>-88</v>
@@ -8283,10 +8298,10 @@
         <v>21</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F129" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G129" s="3">
         <v>-88</v>
@@ -8339,10 +8354,10 @@
         <v>21</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F130" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G130" s="3">
         <v>-88</v>
@@ -8395,10 +8410,10 @@
         <v>21</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>14</v>
+        <v>162</v>
       </c>
       <c r="G131" s="3">
         <v>-88</v>

</xml_diff>